<commit_message>
First row/column are now freezed
</commit_message>
<xml_diff>
--- a/xslx_output_sample.xlsx
+++ b/xslx_output_sample.xlsx
@@ -419,7 +419,10 @@
   <dimension ref="A1:U68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -606,13 +609,13 @@
         <v>34</v>
       </c>
       <c r="S2" t="n">
-        <v>5119</v>
+        <v>5120</v>
       </c>
       <c r="T2" t="n">
         <v>457</v>
       </c>
       <c r="U2" t="n">
-        <v>0.08927499999999999</v>
+        <v>0.089258</v>
       </c>
     </row>
     <row r="3">
@@ -622,40 +625,40 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C3" t="n">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D3" t="n">
-        <v>419</v>
+        <v>466</v>
       </c>
       <c r="E3" t="n">
+        <v>12</v>
+      </c>
+      <c r="F3" t="n">
+        <v>25</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L3" t="n">
         <v>11</v>
       </c>
-      <c r="F3" t="n">
-        <v>20</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" t="n">
-        <v>1</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0</v>
-      </c>
-      <c r="L3" t="n">
-        <v>10</v>
-      </c>
       <c r="M3" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="N3" t="n">
         <v>0</v>
@@ -667,19 +670,19 @@
         <v>1</v>
       </c>
       <c r="Q3" t="n">
-        <v>350</v>
+        <v>394</v>
       </c>
       <c r="R3" t="n">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="S3" t="n">
-        <v>20490</v>
+        <v>22486</v>
       </c>
       <c r="T3" t="n">
-        <v>973</v>
+        <v>1095</v>
       </c>
       <c r="U3" t="n">
-        <v>0.047487</v>
+        <v>0.048697</v>
       </c>
     </row>
     <row r="4">
@@ -689,19 +692,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C4" t="n">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D4" t="n">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="E4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F4" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
@@ -719,34 +722,34 @@
         <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M4" t="n">
         <v>1</v>
       </c>
       <c r="N4" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="O4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P4" t="n">
         <v>0</v>
       </c>
       <c r="Q4" t="n">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="R4" t="n">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="S4" t="n">
-        <v>4111</v>
+        <v>3717</v>
       </c>
       <c r="T4" t="n">
-        <v>311</v>
+        <v>270</v>
       </c>
       <c r="U4" t="n">
-        <v>0.075651</v>
+        <v>0.072639</v>
       </c>
     </row>
     <row r="5">
@@ -762,7 +765,7 @@
         <v>45</v>
       </c>
       <c r="D5" t="n">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E5" t="n">
         <v>3</v>
@@ -801,19 +804,19 @@
         <v>2</v>
       </c>
       <c r="Q5" t="n">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="R5" t="n">
         <v>20</v>
       </c>
       <c r="S5" t="n">
-        <v>8497</v>
+        <v>8506</v>
       </c>
       <c r="T5" t="n">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="U5" t="n">
-        <v>0.056255</v>
+        <v>0.056548</v>
       </c>
     </row>
     <row r="6">
@@ -823,64 +826,64 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C6" t="n">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D6" t="n">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E6" t="n">
+        <v>3</v>
+      </c>
+      <c r="F6" t="n">
+        <v>14</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>2</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" t="n">
+        <v>2</v>
+      </c>
+      <c r="M6" t="n">
+        <v>2</v>
+      </c>
+      <c r="N6" t="n">
+        <v>1</v>
+      </c>
+      <c r="O6" t="n">
         <v>4</v>
       </c>
-      <c r="F6" t="n">
-        <v>24</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" t="n">
-        <v>3</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0</v>
-      </c>
-      <c r="K6" t="n">
-        <v>0</v>
-      </c>
-      <c r="L6" t="n">
-        <v>1</v>
-      </c>
-      <c r="M6" t="n">
-        <v>4</v>
-      </c>
-      <c r="N6" t="n">
-        <v>2</v>
-      </c>
-      <c r="O6" t="n">
-        <v>2</v>
-      </c>
       <c r="P6" t="n">
         <v>0</v>
       </c>
       <c r="Q6" t="n">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="R6" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="S6" t="n">
-        <v>7345</v>
+        <v>7006</v>
       </c>
       <c r="T6" t="n">
-        <v>385</v>
+        <v>338</v>
       </c>
       <c r="U6" t="n">
-        <v>0.052417</v>
+        <v>0.048244</v>
       </c>
     </row>
     <row r="7">
@@ -890,64 +893,64 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C7" t="n">
-        <v>33</v>
+        <v>139</v>
       </c>
       <c r="D7" t="n">
-        <v>46</v>
+        <v>103</v>
       </c>
       <c r="E7" t="n">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F7" t="n">
+        <v>17</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>29</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>16</v>
+      </c>
+      <c r="N7" t="n">
+        <v>5</v>
+      </c>
+      <c r="O7" t="n">
+        <v>34</v>
+      </c>
+      <c r="P7" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>78</v>
+      </c>
+      <c r="R7" t="n">
         <v>9</v>
       </c>
-      <c r="G7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" t="n">
-        <v>6</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" t="n">
-        <v>0</v>
-      </c>
-      <c r="L7" t="n">
-        <v>0</v>
-      </c>
-      <c r="M7" t="n">
-        <v>0</v>
-      </c>
-      <c r="N7" t="n">
-        <v>0</v>
-      </c>
-      <c r="O7" t="n">
-        <v>2</v>
-      </c>
-      <c r="P7" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>21</v>
-      </c>
-      <c r="R7" t="n">
-        <v>5</v>
-      </c>
       <c r="S7" t="n">
-        <v>3121</v>
+        <v>4732</v>
       </c>
       <c r="T7" t="n">
-        <v>144</v>
+        <v>462</v>
       </c>
       <c r="U7" t="n">
-        <v>0.046139</v>
+        <v>0.097633</v>
       </c>
     </row>
     <row r="8">
@@ -957,19 +960,19 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" t="n">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="D8" t="n">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="E8" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F8" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="G8" t="n">
         <v>1</v>
@@ -978,7 +981,7 @@
         <v>2</v>
       </c>
       <c r="I8" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J8" t="n">
         <v>0</v>
@@ -990,31 +993,31 @@
         <v>0</v>
       </c>
       <c r="M8" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="N8" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O8" t="n">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="P8" t="n">
         <v>0</v>
       </c>
       <c r="Q8" t="n">
-        <v>256</v>
+        <v>236</v>
       </c>
       <c r="R8" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S8" t="n">
-        <v>6848</v>
+        <v>6662</v>
       </c>
       <c r="T8" t="n">
-        <v>833</v>
+        <v>777</v>
       </c>
       <c r="U8" t="n">
-        <v>0.121641</v>
+        <v>0.116632</v>
       </c>
     </row>
     <row r="9">
@@ -1075,13 +1078,13 @@
         <v>0</v>
       </c>
       <c r="S9" t="n">
-        <v>11876</v>
+        <v>11883</v>
       </c>
       <c r="T9" t="n">
         <v>39</v>
       </c>
       <c r="U9" t="n">
-        <v>0.003284</v>
+        <v>0.003282</v>
       </c>
     </row>
     <row r="10">
@@ -1136,19 +1139,19 @@
         <v>0</v>
       </c>
       <c r="Q10" t="n">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="R10" t="n">
         <v>16</v>
       </c>
       <c r="S10" t="n">
-        <v>13178</v>
+        <v>13175</v>
       </c>
       <c r="T10" t="n">
-        <v>699</v>
+        <v>702</v>
       </c>
       <c r="U10" t="n">
-        <v>0.053043</v>
+        <v>0.053283</v>
       </c>
     </row>
     <row r="11">
@@ -1158,13 +1161,13 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C11" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D11" t="n">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E11" t="n">
         <v>7</v>
@@ -1197,25 +1200,25 @@
         <v>1</v>
       </c>
       <c r="O11" t="n">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="P11" t="n">
         <v>0</v>
       </c>
       <c r="Q11" t="n">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="R11" t="n">
         <v>11</v>
       </c>
       <c r="S11" t="n">
-        <v>5734</v>
+        <v>5721</v>
       </c>
       <c r="T11" t="n">
-        <v>416</v>
+        <v>408</v>
       </c>
       <c r="U11" t="n">
-        <v>0.07255</v>
+        <v>0.071316</v>
       </c>
     </row>
     <row r="12">
@@ -1270,19 +1273,19 @@
         <v>0</v>
       </c>
       <c r="Q12" t="n">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="R12" t="n">
         <v>10</v>
       </c>
       <c r="S12" t="n">
-        <v>14752</v>
+        <v>14779</v>
       </c>
       <c r="T12" t="n">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="U12" t="n">
-        <v>0.022166</v>
+        <v>0.022194</v>
       </c>
     </row>
     <row r="13">
@@ -1292,64 +1295,64 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C13" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D13" t="n">
-        <v>252</v>
+        <v>263</v>
       </c>
       <c r="E13" t="n">
+        <v>6</v>
+      </c>
+      <c r="F13" t="n">
+        <v>24</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>1</v>
+      </c>
+      <c r="I13" t="n">
+        <v>1</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" t="n">
+        <v>19</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" t="n">
+        <v>2</v>
+      </c>
+      <c r="O13" t="n">
+        <v>15</v>
+      </c>
+      <c r="P13" t="n">
         <v>4</v>
       </c>
-      <c r="F13" t="n">
-        <v>25</v>
-      </c>
-      <c r="G13" t="n">
-        <v>0</v>
-      </c>
-      <c r="H13" t="n">
-        <v>1</v>
-      </c>
-      <c r="I13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J13" t="n">
-        <v>0</v>
-      </c>
-      <c r="K13" t="n">
-        <v>0</v>
-      </c>
-      <c r="L13" t="n">
-        <v>17</v>
-      </c>
-      <c r="M13" t="n">
-        <v>0</v>
-      </c>
-      <c r="N13" t="n">
-        <v>3</v>
-      </c>
-      <c r="O13" t="n">
-        <v>16</v>
-      </c>
-      <c r="P13" t="n">
-        <v>3</v>
-      </c>
       <c r="Q13" t="n">
-        <v>172</v>
+        <v>196</v>
       </c>
       <c r="R13" t="n">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="S13" t="n">
-        <v>13755</v>
+        <v>13972</v>
       </c>
       <c r="T13" t="n">
-        <v>613</v>
+        <v>653</v>
       </c>
       <c r="U13" t="n">
-        <v>0.044566</v>
+        <v>0.046736</v>
       </c>
     </row>
     <row r="14">
@@ -1362,10 +1365,10 @@
         <v>21</v>
       </c>
       <c r="C14" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D14" t="n">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E14" t="n">
         <v>16</v>
@@ -1380,7 +1383,7 @@
         <v>0</v>
       </c>
       <c r="I14" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J14" t="n">
         <v>0</v>
@@ -1404,19 +1407,19 @@
         <v>0</v>
       </c>
       <c r="Q14" t="n">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="R14" t="n">
         <v>15</v>
       </c>
       <c r="S14" t="n">
-        <v>23635</v>
+        <v>23078</v>
       </c>
       <c r="T14" t="n">
-        <v>429</v>
+        <v>419</v>
       </c>
       <c r="U14" t="n">
-        <v>0.018151</v>
+        <v>0.018156</v>
       </c>
     </row>
     <row r="15">
@@ -1426,7 +1429,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C15" t="n">
         <v>35</v>
@@ -1465,25 +1468,25 @@
         <v>5</v>
       </c>
       <c r="O15" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="P15" t="n">
         <v>0</v>
       </c>
       <c r="Q15" t="n">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R15" t="n">
         <v>8</v>
       </c>
       <c r="S15" t="n">
-        <v>7614</v>
+        <v>7601</v>
       </c>
       <c r="T15" t="n">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="U15" t="n">
-        <v>0.069609</v>
+        <v>0.069859</v>
       </c>
     </row>
     <row r="16">
@@ -1544,13 +1547,13 @@
         <v>6</v>
       </c>
       <c r="S16" t="n">
-        <v>19679</v>
+        <v>19697</v>
       </c>
       <c r="T16" t="n">
         <v>152</v>
       </c>
       <c r="U16" t="n">
-        <v>0.007724</v>
+        <v>0.007717</v>
       </c>
     </row>
     <row r="17">
@@ -1627,13 +1630,13 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C18" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D18" t="n">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E18" t="n">
         <v>9</v>
@@ -1672,19 +1675,19 @@
         <v>0</v>
       </c>
       <c r="Q18" t="n">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R18" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S18" t="n">
-        <v>6279</v>
+        <v>6294</v>
       </c>
       <c r="T18" t="n">
         <v>407</v>
       </c>
       <c r="U18" t="n">
-        <v>0.064819</v>
+        <v>0.064665</v>
       </c>
     </row>
     <row r="19">
@@ -1694,19 +1697,19 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C19" t="n">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="D19" t="n">
-        <v>182</v>
+        <v>197</v>
       </c>
       <c r="E19" t="n">
         <v>18</v>
       </c>
       <c r="F19" t="n">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G19" t="n">
         <v>1</v>
@@ -1727,7 +1730,7 @@
         <v>0</v>
       </c>
       <c r="M19" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N19" t="n">
         <v>4</v>
@@ -1739,19 +1742,19 @@
         <v>2</v>
       </c>
       <c r="Q19" t="n">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="R19" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="S19" t="n">
-        <v>6335</v>
+        <v>6365</v>
       </c>
       <c r="T19" t="n">
-        <v>606</v>
+        <v>629</v>
       </c>
       <c r="U19" t="n">
-        <v>0.09565899999999999</v>
+        <v>0.09882199999999999</v>
       </c>
     </row>
     <row r="20">
@@ -1761,19 +1764,19 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C20" t="n">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D20" t="n">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="E20" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F20" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G20" t="n">
         <v>0</v>
@@ -1791,34 +1794,34 @@
         <v>0</v>
       </c>
       <c r="L20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M20" t="n">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="N20" t="n">
         <v>28</v>
       </c>
       <c r="O20" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="P20" t="n">
         <v>0</v>
       </c>
       <c r="Q20" t="n">
-        <v>370</v>
+        <v>307</v>
       </c>
       <c r="R20" t="n">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="S20" t="n">
-        <v>9063</v>
+        <v>8772</v>
       </c>
       <c r="T20" t="n">
-        <v>853</v>
+        <v>753</v>
       </c>
       <c r="U20" t="n">
-        <v>0.09411899999999999</v>
+        <v>0.085841</v>
       </c>
     </row>
     <row r="21">
@@ -1898,10 +1901,10 @@
         <v>43</v>
       </c>
       <c r="C22" t="n">
-        <v>442</v>
+        <v>429</v>
       </c>
       <c r="D22" t="n">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="E22" t="n">
         <v>23</v>
@@ -1916,7 +1919,7 @@
         <v>0</v>
       </c>
       <c r="I22" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J22" t="n">
         <v>0</v>
@@ -1925,13 +1928,13 @@
         <v>0</v>
       </c>
       <c r="L22" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M22" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N22" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="O22" t="n">
         <v>16</v>
@@ -1940,19 +1943,19 @@
         <v>3</v>
       </c>
       <c r="Q22" t="n">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="R22" t="n">
         <v>15</v>
       </c>
       <c r="S22" t="n">
-        <v>19461</v>
+        <v>19051</v>
       </c>
       <c r="T22" t="n">
-        <v>1474</v>
+        <v>1455</v>
       </c>
       <c r="U22" t="n">
-        <v>0.075741</v>
+        <v>0.076374</v>
       </c>
     </row>
     <row r="23">
@@ -1962,19 +1965,19 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C23" t="n">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D23" t="n">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="E23" t="n">
         <v>7</v>
       </c>
       <c r="F23" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G23" t="n">
         <v>1</v>
@@ -2013,13 +2016,13 @@
         <v>41</v>
       </c>
       <c r="S23" t="n">
-        <v>23301</v>
+        <v>23372</v>
       </c>
       <c r="T23" t="n">
-        <v>675</v>
+        <v>682</v>
       </c>
       <c r="U23" t="n">
-        <v>0.028969</v>
+        <v>0.02918</v>
       </c>
     </row>
     <row r="24">
@@ -2080,13 +2083,13 @@
         <v>3</v>
       </c>
       <c r="S24" t="n">
-        <v>16811</v>
+        <v>16825</v>
       </c>
       <c r="T24" t="n">
         <v>166</v>
       </c>
       <c r="U24" t="n">
-        <v>0.009874000000000001</v>
+        <v>0.009866</v>
       </c>
     </row>
     <row r="25">
@@ -2141,19 +2144,19 @@
         <v>0</v>
       </c>
       <c r="Q25" t="n">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="R25" t="n">
         <v>7</v>
       </c>
       <c r="S25" t="n">
-        <v>12456</v>
+        <v>12463</v>
       </c>
       <c r="T25" t="n">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="U25" t="n">
-        <v>0.024004</v>
+        <v>0.024071</v>
       </c>
     </row>
     <row r="26">
@@ -2166,10 +2169,10 @@
         <v>13</v>
       </c>
       <c r="C26" t="n">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D26" t="n">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="E26" t="n">
         <v>9</v>
@@ -2184,7 +2187,7 @@
         <v>0</v>
       </c>
       <c r="I26" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="J26" t="n">
         <v>2</v>
@@ -2208,19 +2211,19 @@
         <v>0</v>
       </c>
       <c r="Q26" t="n">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="R26" t="n">
         <v>23</v>
       </c>
       <c r="S26" t="n">
-        <v>22698</v>
+        <v>22366</v>
       </c>
       <c r="T26" t="n">
-        <v>468</v>
+        <v>456</v>
       </c>
       <c r="U26" t="n">
-        <v>0.020619</v>
+        <v>0.020388</v>
       </c>
     </row>
     <row r="27">
@@ -2300,10 +2303,10 @@
         <v>31</v>
       </c>
       <c r="C28" t="n">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D28" t="n">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="E28" t="n">
         <v>4</v>
@@ -2333,7 +2336,7 @@
         <v>10</v>
       </c>
       <c r="N28" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O28" t="n">
         <v>4</v>
@@ -2342,19 +2345,19 @@
         <v>0</v>
       </c>
       <c r="Q28" t="n">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="R28" t="n">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="S28" t="n">
-        <v>10763</v>
+        <v>10839</v>
       </c>
       <c r="T28" t="n">
-        <v>842</v>
+        <v>851</v>
       </c>
       <c r="U28" t="n">
-        <v>0.07823099999999999</v>
+        <v>0.078513</v>
       </c>
     </row>
     <row r="29">
@@ -2364,19 +2367,19 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C29" t="n">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D29" t="n">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E29" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F29" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G29" t="n">
         <v>0</v>
@@ -2385,7 +2388,7 @@
         <v>0</v>
       </c>
       <c r="I29" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J29" t="n">
         <v>4</v>
@@ -2397,31 +2400,31 @@
         <v>1</v>
       </c>
       <c r="M29" t="n">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="N29" t="n">
         <v>3</v>
       </c>
       <c r="O29" t="n">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="P29" t="n">
         <v>1</v>
       </c>
       <c r="Q29" t="n">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="R29" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S29" t="n">
-        <v>6887</v>
+        <v>6489</v>
       </c>
       <c r="T29" t="n">
-        <v>249</v>
+        <v>234</v>
       </c>
       <c r="U29" t="n">
-        <v>0.036155</v>
+        <v>0.036061</v>
       </c>
     </row>
     <row r="30">
@@ -2437,7 +2440,7 @@
         <v>20</v>
       </c>
       <c r="D30" t="n">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="E30" t="n">
         <v>5</v>
@@ -2476,19 +2479,19 @@
         <v>0</v>
       </c>
       <c r="Q30" t="n">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="R30" t="n">
         <v>62</v>
       </c>
       <c r="S30" t="n">
-        <v>19213</v>
+        <v>19396</v>
       </c>
       <c r="T30" t="n">
-        <v>501</v>
+        <v>508</v>
       </c>
       <c r="U30" t="n">
-        <v>0.026076</v>
+        <v>0.026191</v>
       </c>
     </row>
     <row r="31">
@@ -2501,10 +2504,10 @@
         <v>29</v>
       </c>
       <c r="C31" t="n">
-        <v>482</v>
+        <v>464</v>
       </c>
       <c r="D31" t="n">
-        <v>397</v>
+        <v>353</v>
       </c>
       <c r="E31" t="n">
         <v>7</v>
@@ -2519,7 +2522,7 @@
         <v>0</v>
       </c>
       <c r="I31" t="n">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="J31" t="n">
         <v>0</v>
@@ -2531,31 +2534,31 @@
         <v>3</v>
       </c>
       <c r="M31" t="n">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="N31" t="n">
         <v>11</v>
       </c>
       <c r="O31" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="P31" t="n">
         <v>4</v>
       </c>
       <c r="Q31" t="n">
-        <v>454</v>
+        <v>458</v>
       </c>
       <c r="R31" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S31" t="n">
-        <v>13293</v>
+        <v>13215</v>
       </c>
       <c r="T31" t="n">
-        <v>1555</v>
+        <v>1519</v>
       </c>
       <c r="U31" t="n">
-        <v>0.116979</v>
+        <v>0.114945</v>
       </c>
     </row>
     <row r="32">
@@ -2565,19 +2568,19 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C32" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D32" t="n">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="E32" t="n">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="F32" t="n">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G32" t="n">
         <v>0</v>
@@ -2586,7 +2589,7 @@
         <v>0</v>
       </c>
       <c r="I32" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J32" t="n">
         <v>0</v>
@@ -2595,7 +2598,7 @@
         <v>2</v>
       </c>
       <c r="L32" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="M32" t="n">
         <v>6</v>
@@ -2610,19 +2613,19 @@
         <v>0</v>
       </c>
       <c r="Q32" t="n">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="R32" t="n">
         <v>24</v>
       </c>
       <c r="S32" t="n">
-        <v>6434</v>
+        <v>6865</v>
       </c>
       <c r="T32" t="n">
-        <v>490</v>
+        <v>514</v>
       </c>
       <c r="U32" t="n">
-        <v>0.076158</v>
+        <v>0.074873</v>
       </c>
     </row>
     <row r="33">
@@ -2632,13 +2635,13 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C33" t="n">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D33" t="n">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E33" t="n">
         <v>7</v>
@@ -2671,25 +2674,25 @@
         <v>0</v>
       </c>
       <c r="O33" t="n">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="P33" t="n">
         <v>11</v>
       </c>
       <c r="Q33" t="n">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="R33" t="n">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="S33" t="n">
-        <v>5399</v>
+        <v>5280</v>
       </c>
       <c r="T33" t="n">
-        <v>500</v>
+        <v>485</v>
       </c>
       <c r="U33" t="n">
-        <v>0.09261</v>
+        <v>0.09185599999999999</v>
       </c>
     </row>
     <row r="34">
@@ -2705,7 +2708,7 @@
         <v>12</v>
       </c>
       <c r="D34" t="n">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="E34" t="n">
         <v>4</v>
@@ -2744,19 +2747,19 @@
         <v>0</v>
       </c>
       <c r="Q34" t="n">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="R34" t="n">
         <v>13</v>
       </c>
       <c r="S34" t="n">
-        <v>18051</v>
+        <v>18179</v>
       </c>
       <c r="T34" t="n">
-        <v>487</v>
+        <v>493</v>
       </c>
       <c r="U34" t="n">
-        <v>0.026979</v>
+        <v>0.027119</v>
       </c>
     </row>
     <row r="35">
@@ -2772,13 +2775,13 @@
         <v>80</v>
       </c>
       <c r="D35" t="n">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="E35" t="n">
         <v>20</v>
       </c>
       <c r="F35" t="n">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G35" t="n">
         <v>4</v>
@@ -2817,13 +2820,13 @@
         <v>39</v>
       </c>
       <c r="S35" t="n">
-        <v>22721</v>
+        <v>22829</v>
       </c>
       <c r="T35" t="n">
-        <v>1034</v>
+        <v>1036</v>
       </c>
       <c r="U35" t="n">
-        <v>0.045509</v>
+        <v>0.045381</v>
       </c>
     </row>
     <row r="36">
@@ -2833,19 +2836,19 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C36" t="n">
         <v>17</v>
       </c>
       <c r="D36" t="n">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E36" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F36" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G36" t="n">
         <v>0</v>
@@ -2875,22 +2878,22 @@
         <v>2</v>
       </c>
       <c r="P36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q36" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="R36" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="S36" t="n">
-        <v>5794</v>
+        <v>5870</v>
       </c>
       <c r="T36" t="n">
-        <v>232</v>
+        <v>239</v>
       </c>
       <c r="U36" t="n">
-        <v>0.040041</v>
+        <v>0.040716</v>
       </c>
     </row>
     <row r="37">
@@ -2945,19 +2948,19 @@
         <v>1</v>
       </c>
       <c r="Q37" t="n">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="R37" t="n">
         <v>21</v>
       </c>
       <c r="S37" t="n">
-        <v>10475</v>
+        <v>10447</v>
       </c>
       <c r="T37" t="n">
-        <v>675</v>
+        <v>677</v>
       </c>
       <c r="U37" t="n">
-        <v>0.064439</v>
+        <v>0.064803</v>
       </c>
     </row>
     <row r="38">
@@ -2973,7 +2976,7 @@
         <v>39</v>
       </c>
       <c r="D38" t="n">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="E38" t="n">
         <v>5</v>
@@ -3012,19 +3015,19 @@
         <v>0</v>
       </c>
       <c r="Q38" t="n">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="R38" t="n">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="S38" t="n">
-        <v>6569</v>
+        <v>6634</v>
       </c>
       <c r="T38" t="n">
-        <v>789</v>
+        <v>794</v>
       </c>
       <c r="U38" t="n">
-        <v>0.12011</v>
+        <v>0.119686</v>
       </c>
     </row>
     <row r="39">
@@ -3037,16 +3040,16 @@
         <v>11</v>
       </c>
       <c r="C39" t="n">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D39" t="n">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="E39" t="n">
         <v>0</v>
       </c>
       <c r="F39" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G39" t="n">
         <v>2</v>
@@ -3055,7 +3058,7 @@
         <v>0</v>
       </c>
       <c r="I39" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J39" t="n">
         <v>2</v>
@@ -3073,25 +3076,25 @@
         <v>3</v>
       </c>
       <c r="O39" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="P39" t="n">
         <v>0</v>
       </c>
       <c r="Q39" t="n">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="R39" t="n">
         <v>7</v>
       </c>
       <c r="S39" t="n">
-        <v>7216</v>
+        <v>7130</v>
       </c>
       <c r="T39" t="n">
-        <v>683</v>
+        <v>675</v>
       </c>
       <c r="U39" t="n">
-        <v>0.094651</v>
+        <v>0.09467</v>
       </c>
     </row>
     <row r="40">
@@ -3101,10 +3104,10 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C40" t="n">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D40" t="n">
         <v>390</v>
@@ -3146,19 +3149,19 @@
         <v>2</v>
       </c>
       <c r="Q40" t="n">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="R40" t="n">
         <v>36</v>
       </c>
       <c r="S40" t="n">
-        <v>10761</v>
+        <v>10769</v>
       </c>
       <c r="T40" t="n">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="U40" t="n">
-        <v>0.09329999999999999</v>
+        <v>0.093416</v>
       </c>
     </row>
     <row r="41">
@@ -3219,13 +3222,13 @@
         <v>20</v>
       </c>
       <c r="S41" t="n">
-        <v>8582</v>
+        <v>8591</v>
       </c>
       <c r="T41" t="n">
         <v>505</v>
       </c>
       <c r="U41" t="n">
-        <v>0.058844</v>
+        <v>0.058782</v>
       </c>
     </row>
     <row r="42">
@@ -3286,13 +3289,13 @@
         <v>2</v>
       </c>
       <c r="S42" t="n">
-        <v>5296</v>
+        <v>5297</v>
       </c>
       <c r="T42" t="n">
         <v>114</v>
       </c>
       <c r="U42" t="n">
-        <v>0.021526</v>
+        <v>0.021522</v>
       </c>
     </row>
     <row r="43">
@@ -3302,64 +3305,64 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C43" t="n">
-        <v>1126</v>
+        <v>716</v>
       </c>
       <c r="D43" t="n">
-        <v>587</v>
+        <v>467</v>
       </c>
       <c r="E43" t="n">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="F43" t="n">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="G43" t="n">
+        <v>3</v>
+      </c>
+      <c r="H43" t="n">
+        <v>2</v>
+      </c>
+      <c r="I43" t="n">
+        <v>232</v>
+      </c>
+      <c r="J43" t="n">
+        <v>0</v>
+      </c>
+      <c r="K43" t="n">
+        <v>1</v>
+      </c>
+      <c r="L43" t="n">
         <v>5</v>
       </c>
-      <c r="H43" t="n">
-        <v>1</v>
-      </c>
-      <c r="I43" t="n">
-        <v>245</v>
-      </c>
-      <c r="J43" t="n">
-        <v>0</v>
-      </c>
-      <c r="K43" t="n">
-        <v>1</v>
-      </c>
-      <c r="L43" t="n">
-        <v>7</v>
-      </c>
       <c r="M43" t="n">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="N43" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="O43" t="n">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P43" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q43" t="n">
-        <v>455</v>
+        <v>415</v>
       </c>
       <c r="R43" t="n">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="S43" t="n">
-        <v>12360</v>
+        <v>10064</v>
       </c>
       <c r="T43" t="n">
-        <v>2876</v>
+        <v>2235</v>
       </c>
       <c r="U43" t="n">
-        <v>0.232686</v>
+        <v>0.222079</v>
       </c>
     </row>
     <row r="44">
@@ -3414,19 +3417,19 @@
         <v>0</v>
       </c>
       <c r="Q44" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R44" t="n">
         <v>0</v>
       </c>
       <c r="S44" t="n">
-        <v>1359</v>
+        <v>1367</v>
       </c>
       <c r="T44" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="U44" t="n">
-        <v>0.008094</v>
+        <v>0.008777999999999999</v>
       </c>
     </row>
     <row r="45">
@@ -3436,19 +3439,19 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C45" t="n">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D45" t="n">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E45" t="n">
         <v>9</v>
       </c>
       <c r="F45" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G45" t="n">
         <v>0</v>
@@ -3475,25 +3478,25 @@
         <v>2</v>
       </c>
       <c r="O45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P45" t="n">
         <v>1</v>
       </c>
       <c r="Q45" t="n">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="R45" t="n">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="S45" t="n">
-        <v>4858</v>
+        <v>5053</v>
       </c>
       <c r="T45" t="n">
-        <v>484</v>
+        <v>477</v>
       </c>
       <c r="U45" t="n">
-        <v>0.099629</v>
+        <v>0.094399</v>
       </c>
     </row>
     <row r="46">
@@ -3506,7 +3509,7 @@
         <v>3</v>
       </c>
       <c r="C46" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D46" t="n">
         <v>20</v>
@@ -3515,7 +3518,7 @@
         <v>0</v>
       </c>
       <c r="F46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G46" t="n">
         <v>0</v>
@@ -3548,19 +3551,19 @@
         <v>0</v>
       </c>
       <c r="Q46" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="R46" t="n">
         <v>2</v>
       </c>
       <c r="S46" t="n">
-        <v>2530</v>
+        <v>2498</v>
       </c>
       <c r="T46" t="n">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="U46" t="n">
-        <v>0.022134</v>
+        <v>0.020817</v>
       </c>
     </row>
     <row r="47">
@@ -3615,19 +3618,19 @@
         <v>0</v>
       </c>
       <c r="Q47" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="R47" t="n">
         <v>2</v>
       </c>
       <c r="S47" t="n">
-        <v>16197</v>
+        <v>16242</v>
       </c>
       <c r="T47" t="n">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="U47" t="n">
-        <v>0.013336</v>
+        <v>0.01336</v>
       </c>
     </row>
     <row r="48">
@@ -3643,7 +3646,7 @@
         <v>31</v>
       </c>
       <c r="D48" t="n">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E48" t="n">
         <v>4</v>
@@ -3682,19 +3685,19 @@
         <v>0</v>
       </c>
       <c r="Q48" t="n">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="R48" t="n">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S48" t="n">
-        <v>5372</v>
+        <v>5382</v>
       </c>
       <c r="T48" t="n">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="U48" t="n">
-        <v>0.100149</v>
+        <v>0.099777</v>
       </c>
     </row>
     <row r="49">
@@ -3713,7 +3716,7 @@
         <v>210</v>
       </c>
       <c r="E49" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F49" t="n">
         <v>58</v>
@@ -3755,13 +3758,13 @@
         <v>58</v>
       </c>
       <c r="S49" t="n">
-        <v>14366</v>
+        <v>14468</v>
       </c>
       <c r="T49" t="n">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="U49" t="n">
-        <v>0.047195</v>
+        <v>0.046931</v>
       </c>
     </row>
     <row r="50">
@@ -3771,13 +3774,13 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C50" t="n">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D50" t="n">
-        <v>132</v>
+        <v>145</v>
       </c>
       <c r="E50" t="n">
         <v>2</v>
@@ -3795,7 +3798,7 @@
         <v>1</v>
       </c>
       <c r="J50" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K50" t="n">
         <v>0</v>
@@ -3810,25 +3813,25 @@
         <v>1</v>
       </c>
       <c r="O50" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="P50" t="n">
         <v>16</v>
       </c>
       <c r="Q50" t="n">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="R50" t="n">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="S50" t="n">
-        <v>11974</v>
+        <v>12560</v>
       </c>
       <c r="T50" t="n">
-        <v>441</v>
+        <v>473</v>
       </c>
       <c r="U50" t="n">
-        <v>0.03683</v>
+        <v>0.037659</v>
       </c>
     </row>
     <row r="51">
@@ -3889,13 +3892,13 @@
         <v>13</v>
       </c>
       <c r="S51" t="n">
-        <v>17373</v>
+        <v>17377</v>
       </c>
       <c r="T51" t="n">
         <v>823</v>
       </c>
       <c r="U51" t="n">
-        <v>0.047372</v>
+        <v>0.047361</v>
       </c>
     </row>
     <row r="52">
@@ -3908,16 +3911,16 @@
         <v>20</v>
       </c>
       <c r="C52" t="n">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D52" t="n">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="E52" t="n">
         <v>10</v>
       </c>
       <c r="F52" t="n">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G52" t="n">
         <v>0</v>
@@ -3938,7 +3941,7 @@
         <v>3</v>
       </c>
       <c r="M52" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="N52" t="n">
         <v>0</v>
@@ -3953,16 +3956,16 @@
         <v>385</v>
       </c>
       <c r="R52" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S52" t="n">
-        <v>17493</v>
+        <v>17495</v>
       </c>
       <c r="T52" t="n">
-        <v>945</v>
+        <v>926</v>
       </c>
       <c r="U52" t="n">
-        <v>0.054022</v>
+        <v>0.052929</v>
       </c>
     </row>
     <row r="53">
@@ -3978,7 +3981,7 @@
         <v>10</v>
       </c>
       <c r="D53" t="n">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="E53" t="n">
         <v>8</v>
@@ -4017,19 +4020,19 @@
         <v>1</v>
       </c>
       <c r="Q53" t="n">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="R53" t="n">
         <v>16</v>
       </c>
       <c r="S53" t="n">
-        <v>17990</v>
+        <v>18066</v>
       </c>
       <c r="T53" t="n">
-        <v>658</v>
+        <v>660</v>
       </c>
       <c r="U53" t="n">
-        <v>0.036576</v>
+        <v>0.036533</v>
       </c>
     </row>
     <row r="54">
@@ -4084,19 +4087,19 @@
         <v>1</v>
       </c>
       <c r="Q54" t="n">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="R54" t="n">
         <v>27</v>
       </c>
       <c r="S54" t="n">
-        <v>6351</v>
+        <v>6365</v>
       </c>
       <c r="T54" t="n">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="U54" t="n">
-        <v>0.09415800000000001</v>
+        <v>0.094108</v>
       </c>
     </row>
     <row r="55">
@@ -4106,19 +4109,19 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C55" t="n">
-        <v>677</v>
+        <v>679</v>
       </c>
       <c r="D55" t="n">
-        <v>212</v>
+        <v>219</v>
       </c>
       <c r="E55" t="n">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="F55" t="n">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="G55" t="n">
         <v>0</v>
@@ -4127,7 +4130,7 @@
         <v>2</v>
       </c>
       <c r="I55" t="n">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="J55" t="n">
         <v>0</v>
@@ -4136,34 +4139,34 @@
         <v>0</v>
       </c>
       <c r="L55" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M55" t="n">
         <v>16</v>
       </c>
       <c r="N55" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O55" t="n">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="P55" t="n">
         <v>3</v>
       </c>
       <c r="Q55" t="n">
-        <v>207</v>
+        <v>253</v>
       </c>
       <c r="R55" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="S55" t="n">
-        <v>7423</v>
+        <v>7987</v>
       </c>
       <c r="T55" t="n">
-        <v>1272</v>
+        <v>1324</v>
       </c>
       <c r="U55" t="n">
-        <v>0.171359</v>
+        <v>0.165769</v>
       </c>
     </row>
     <row r="56">
@@ -4224,13 +4227,13 @@
         <v>15</v>
       </c>
       <c r="S56" t="n">
-        <v>25084</v>
+        <v>25110</v>
       </c>
       <c r="T56" t="n">
         <v>503</v>
       </c>
       <c r="U56" t="n">
-        <v>0.020053</v>
+        <v>0.020032</v>
       </c>
     </row>
     <row r="57">
@@ -4240,28 +4243,28 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="C57" t="n">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="D57" t="n">
-        <v>466</v>
+        <v>575</v>
       </c>
       <c r="E57" t="n">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F57" t="n">
-        <v>114</v>
+        <v>133</v>
       </c>
       <c r="G57" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H57" t="n">
         <v>0</v>
       </c>
       <c r="I57" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J57" t="n">
         <v>0</v>
@@ -4270,34 +4273,34 @@
         <v>0</v>
       </c>
       <c r="L57" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M57" t="n">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="N57" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O57" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="P57" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q57" t="n">
-        <v>492</v>
+        <v>565</v>
       </c>
       <c r="R57" t="n">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="S57" t="n">
-        <v>16030</v>
+        <v>19068</v>
       </c>
       <c r="T57" t="n">
-        <v>1417</v>
+        <v>1663</v>
       </c>
       <c r="U57" t="n">
-        <v>0.088397</v>
+        <v>0.087214</v>
       </c>
     </row>
     <row r="58">
@@ -4307,19 +4310,19 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>202</v>
+        <v>219</v>
       </c>
       <c r="C58" t="n">
-        <v>378</v>
+        <v>409</v>
       </c>
       <c r="D58" t="n">
-        <v>1638</v>
+        <v>1749</v>
       </c>
       <c r="E58" t="n">
-        <v>185</v>
+        <v>194</v>
       </c>
       <c r="F58" t="n">
-        <v>306</v>
+        <v>333</v>
       </c>
       <c r="G58" t="n">
         <v>3</v>
@@ -4328,10 +4331,10 @@
         <v>0</v>
       </c>
       <c r="I58" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="J58" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K58" t="n">
         <v>4</v>
@@ -4340,31 +4343,31 @@
         <v>20</v>
       </c>
       <c r="M58" t="n">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="N58" t="n">
         <v>13</v>
       </c>
       <c r="O58" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P58" t="n">
         <v>0</v>
       </c>
       <c r="Q58" t="n">
-        <v>1599</v>
+        <v>1666</v>
       </c>
       <c r="R58" t="n">
-        <v>281</v>
+        <v>308</v>
       </c>
       <c r="S58" t="n">
-        <v>81537</v>
+        <v>86223</v>
       </c>
       <c r="T58" t="n">
-        <v>4765</v>
+        <v>5059</v>
       </c>
       <c r="U58" t="n">
-        <v>0.05844</v>
+        <v>0.058673</v>
       </c>
     </row>
     <row r="59">
@@ -4374,16 +4377,16 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C59" t="n">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D59" t="n">
-        <v>214</v>
+        <v>251</v>
       </c>
       <c r="E59" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F59" t="n">
         <v>15</v>
@@ -4410,7 +4413,7 @@
         <v>3</v>
       </c>
       <c r="N59" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O59" t="n">
         <v>4</v>
@@ -4419,19 +4422,19 @@
         <v>0</v>
       </c>
       <c r="Q59" t="n">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="R59" t="n">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="S59" t="n">
-        <v>8468</v>
+        <v>8763</v>
       </c>
       <c r="T59" t="n">
-        <v>530</v>
+        <v>580</v>
       </c>
       <c r="U59" t="n">
-        <v>0.06258900000000001</v>
+        <v>0.066187</v>
       </c>
     </row>
     <row r="60">
@@ -4486,19 +4489,19 @@
         <v>0</v>
       </c>
       <c r="Q60" t="n">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="R60" t="n">
         <v>7</v>
       </c>
       <c r="S60" t="n">
-        <v>7463</v>
+        <v>7506</v>
       </c>
       <c r="T60" t="n">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="U60" t="n">
-        <v>0.045826</v>
+        <v>0.045697</v>
       </c>
     </row>
     <row r="61">
@@ -4508,19 +4511,19 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C61" t="n">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="D61" t="n">
-        <v>352</v>
+        <v>277</v>
       </c>
       <c r="E61" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F61" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G61" t="n">
         <v>0</v>
@@ -4529,19 +4532,19 @@
         <v>0</v>
       </c>
       <c r="I61" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J61" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="K61" t="n">
         <v>0</v>
       </c>
       <c r="L61" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M61" t="n">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="N61" t="n">
         <v>0</v>
@@ -4553,19 +4556,19 @@
         <v>0</v>
       </c>
       <c r="Q61" t="n">
-        <v>337</v>
+        <v>260</v>
       </c>
       <c r="R61" t="n">
-        <v>130</v>
+        <v>89</v>
       </c>
       <c r="S61" t="n">
-        <v>20766</v>
+        <v>16443</v>
       </c>
       <c r="T61" t="n">
-        <v>1001</v>
+        <v>760</v>
       </c>
       <c r="U61" t="n">
-        <v>0.048204</v>
+        <v>0.04622</v>
       </c>
     </row>
     <row r="62">
@@ -4626,7 +4629,7 @@
         <v>5</v>
       </c>
       <c r="S62" t="n">
-        <v>20085</v>
+        <v>20086</v>
       </c>
       <c r="T62" t="n">
         <v>178</v>
@@ -4693,13 +4696,13 @@
         <v>10</v>
       </c>
       <c r="S63" t="n">
-        <v>14854</v>
+        <v>14866</v>
       </c>
       <c r="T63" t="n">
         <v>305</v>
       </c>
       <c r="U63" t="n">
-        <v>0.020533</v>
+        <v>0.020517</v>
       </c>
     </row>
     <row r="64">
@@ -4748,7 +4751,7 @@
         <v>4</v>
       </c>
       <c r="O64" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="P64" t="n">
         <v>27</v>
@@ -4760,13 +4763,13 @@
         <v>54</v>
       </c>
       <c r="S64" t="n">
-        <v>20006</v>
+        <v>20033</v>
       </c>
       <c r="T64" t="n">
-        <v>1258</v>
+        <v>1259</v>
       </c>
       <c r="U64" t="n">
-        <v>0.06288100000000001</v>
+        <v>0.062846</v>
       </c>
     </row>
     <row r="65">
@@ -4827,13 +4830,13 @@
         <v>0</v>
       </c>
       <c r="S65" t="n">
-        <v>1173</v>
+        <v>1175</v>
       </c>
       <c r="T65" t="n">
         <v>29</v>
       </c>
       <c r="U65" t="n">
-        <v>0.024723</v>
+        <v>0.024681</v>
       </c>
     </row>
     <row r="66">
@@ -4846,16 +4849,16 @@
         <v>18</v>
       </c>
       <c r="C66" t="n">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D66" t="n">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="E66" t="n">
         <v>2</v>
       </c>
       <c r="F66" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G66" t="n">
         <v>0</v>
@@ -4888,19 +4891,19 @@
         <v>1</v>
       </c>
       <c r="Q66" t="n">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="R66" t="n">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="S66" t="n">
-        <v>7229</v>
+        <v>7391</v>
       </c>
       <c r="T66" t="n">
-        <v>545</v>
+        <v>561</v>
       </c>
       <c r="U66" t="n">
-        <v>0.075391</v>
+        <v>0.075903</v>
       </c>
     </row>
     <row r="67">
@@ -4916,7 +4919,7 @@
         <v>49</v>
       </c>
       <c r="D67" t="n">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="E67" t="n">
         <v>6</v>
@@ -4943,7 +4946,7 @@
         <v>4</v>
       </c>
       <c r="M67" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N67" t="n">
         <v>0</v>
@@ -4961,13 +4964,13 @@
         <v>22</v>
       </c>
       <c r="S67" t="n">
-        <v>12029</v>
+        <v>12038</v>
       </c>
       <c r="T67" t="n">
-        <v>1076</v>
+        <v>1078</v>
       </c>
       <c r="U67" t="n">
-        <v>0.08945</v>
+        <v>0.08955</v>
       </c>
     </row>
     <row r="68">
@@ -5028,13 +5031,13 @@
         <v>14</v>
       </c>
       <c r="S68" t="n">
-        <v>16716</v>
+        <v>16719</v>
       </c>
       <c r="T68" t="n">
         <v>296</v>
       </c>
       <c r="U68" t="n">
-        <v>0.017708</v>
+        <v>0.017704</v>
       </c>
     </row>
   </sheetData>

</xml_diff>